<commit_message>
progression excel + script insertion donnees stagiaires
</commit_message>
<xml_diff>
--- a/persistance_des_données/mettre_en_place_une_base_de_donnees/exercice_marque_modele_voiture/Marque Modele.xlsx
+++ b/persistance_des_données/mettre_en_place_une_base_de_donnees/exercice_marque_modele_voiture/Marque Modele.xlsx
@@ -1867,7 +1867,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -1876,6 +1876,7 @@
     <col bestFit="1" customWidth="1" min="1" max="1" width="22.109375"/>
     <col bestFit="1" customWidth="1" min="2" max="2" width="14.109375"/>
     <col bestFit="1" min="5" max="5" width="13.7109375"/>
+    <col bestFit="1" min="7" max="7" width="20.57421875"/>
     <col bestFit="1" min="9" max="9" width="74.00390625"/>
     <col bestFit="1" min="10" max="10" width="13.28125"/>
     <col bestFit="1" min="12" max="12" width="67.140625"/>
@@ -1942,7 +1943,7 @@
       </c>
       <c r="O2" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-06-jj</v>
+        <v>-05-jj</v>
       </c>
     </row>
     <row r="3">
@@ -1984,7 +1985,7 @@
       </c>
       <c r="O3" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-11-jj</v>
+        <v>-09-jj</v>
       </c>
     </row>
     <row r="4">
@@ -2068,7 +2069,7 @@
       </c>
       <c r="O5" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-07-jj</v>
+        <v>-08-jj</v>
       </c>
     </row>
     <row r="6">
@@ -2110,7 +2111,7 @@
       </c>
       <c r="O6" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-06-jj</v>
+        <v>-05-jj</v>
       </c>
     </row>
     <row r="7">
@@ -2152,7 +2153,7 @@
       </c>
       <c r="O7" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-01-jj</v>
+        <v>-06-jj</v>
       </c>
     </row>
     <row r="8">
@@ -2194,7 +2195,7 @@
       </c>
       <c r="O8" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-01-jj</v>
+        <v>-05-jj</v>
       </c>
     </row>
     <row r="9">
@@ -2236,7 +2237,7 @@
       </c>
       <c r="O9" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-07-jj</v>
+        <v>-08-jj</v>
       </c>
     </row>
     <row r="10">
@@ -2278,7 +2279,7 @@
       </c>
       <c r="O10" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-01-jj</v>
+        <v>-12-jj</v>
       </c>
     </row>
     <row r="11">
@@ -2320,7 +2321,7 @@
       </c>
       <c r="O11" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-03-jj</v>
+        <v>-07-jj</v>
       </c>
     </row>
     <row r="12">
@@ -2362,7 +2363,7 @@
       </c>
       <c r="O12" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-08-jj</v>
+        <v>-01-jj</v>
       </c>
     </row>
     <row r="13">
@@ -2404,7 +2405,7 @@
       </c>
       <c r="O13" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-08-jj</v>
+        <v>-04-jj</v>
       </c>
     </row>
     <row r="14">
@@ -2488,7 +2489,7 @@
       </c>
       <c r="O15" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-02-jj</v>
+        <v>-06-jj</v>
       </c>
     </row>
     <row r="16">
@@ -2530,7 +2531,7 @@
       </c>
       <c r="O16" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-05-jj</v>
+        <v>-06-jj</v>
       </c>
     </row>
     <row r="17">
@@ -2572,7 +2573,7 @@
       </c>
       <c r="O17" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-03-jj</v>
+        <v>-06-jj</v>
       </c>
     </row>
     <row r="18">
@@ -2656,7 +2657,7 @@
       </c>
       <c r="O19" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-07-jj</v>
+        <v>-12-jj</v>
       </c>
     </row>
     <row r="20">
@@ -2698,7 +2699,7 @@
       </c>
       <c r="O20" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-03-jj</v>
+        <v>-05-jj</v>
       </c>
     </row>
     <row r="21">
@@ -2740,7 +2741,7 @@
       </c>
       <c r="O21" t="str">
         <f ca="1">TEXT(DATE(2020,1,1)+RANDBETWEEN(0,1000),"aaaa-mm-jj")</f>
-        <v>-02-jj</v>
+        <v>-07-jj</v>
       </c>
     </row>
     <row r="22">

</xml_diff>